<commit_message>
update property images and enhance carousel functionality
</commit_message>
<xml_diff>
--- a/propiedades.xlsx
+++ b/propiedades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef6e17dde6493340/Escritorio/Inmobiliaria/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{82578868-331C-4E77-85D7-C74C47BFD264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9FF8E81-7BF1-4495-A549-E689B04CE290}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{82578868-331C-4E77-85D7-C74C47BFD264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{924A68BD-C79C-41D2-9F9C-E9006792C8EF}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{2B61FF61-0429-4616-9C70-6CECAA32CFE0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2B61FF61-0429-4616-9C70-6CECAA32CFE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Propiedades" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>ID</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Carlos Paz</t>
   </si>
   <si>
-    <t>https://via.placeholder.com/600x400/667eea/ffffff?text=Depto+Moderno+1</t>
-  </si>
-  <si>
     <t>Casa con Jardín</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>Calamuchita</t>
   </si>
   <si>
-    <t>https://via.placeholder.com/600x400/48bb78/ffffff?text=Casa+Jardin+1</t>
-  </si>
-  <si>
     <t>alquiler</t>
   </si>
   <si>
@@ -173,14 +167,17 @@
     <t>Jujuy</t>
   </si>
   <si>
-    <t>casa1.png, casa2.png, casa3.png</t>
+    <t>casa1.jpg, casa2.jpg, casa3.jpg</t>
+  </si>
+  <si>
+    <t>1.jpg, 2.jpg, 3.jpg, 4.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +198,20 @@
       <color rgb="FFCCCCCC"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -226,17 +237,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -621,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533FFC6F-FA3C-4F72-887B-786341E0AB76}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,8 +723,8 @@
       <c r="I2">
         <v>2</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>45</v>
+      <c r="J2" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="K2" s="2"/>
     </row>
@@ -739,8 +756,8 @@
       <c r="I3">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
-        <v>21</v>
+      <c r="J3" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -754,16 +771,16 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
         <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
       </c>
       <c r="F4">
         <v>350000</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4">
         <v>4</v>
@@ -772,7 +789,7 @@
         <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -783,13 +800,13 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
         <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
       </c>
       <c r="F5">
         <v>45000</v>
@@ -804,7 +821,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -812,22 +829,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F6">
         <v>2500000</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -836,7 +853,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -844,16 +861,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F7">
         <v>95000</v>
@@ -868,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -879,19 +896,19 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F8">
         <v>80000</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8">
         <v>3</v>
@@ -900,7 +917,7 @@
         <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -914,16 +931,16 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F9">
         <v>50000</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H9">
         <v>2</v>

</xml_diff>